<commit_message>
revised project based on review
</commit_message>
<xml_diff>
--- a/AB_Project_Results.xlsx
+++ b/AB_Project_Results.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Udacity\DA\P7\Final_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="930" yWindow="0" windowWidth="22515" windowHeight="7140"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Control" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Experiment" sheetId="2" r:id="rId4"/>
+    <sheet name="Control" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiment" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -153,29 +161,57 @@
   </si>
   <si>
     <t>Sun, Nov 16</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>CTP</t>
+  </si>
+  <si>
+    <t>CI-</t>
+  </si>
+  <si>
+    <t>CI+</t>
+  </si>
+  <si>
+    <t>Pcont</t>
+  </si>
+  <si>
+    <t>Pexp</t>
+  </si>
+  <si>
+    <t>SEcont</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -184,61 +220,351 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -261,97 +587,97 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>7723.0</v>
+        <v>7723</v>
       </c>
       <c r="C2" s="3">
-        <v>687.0</v>
+        <v>687</v>
       </c>
       <c r="D2" s="3">
-        <v>134.0</v>
+        <v>134</v>
       </c>
       <c r="E2" s="3">
-        <v>70.0</v>
-      </c>
-      <c r="G2" t="str">
+        <v>70</v>
+      </c>
+      <c r="G2">
         <f>Experiment!D2-D2</f>
         <v>-29</v>
       </c>
       <c r="H2" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="str">
+      <c r="J2">
         <f>Experiment!E2-E2</f>
         <v>-36</v>
       </c>
       <c r="K2" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3">
-        <v>9102.0</v>
+        <v>9102</v>
       </c>
       <c r="C3" s="3">
-        <v>779.0</v>
+        <v>779</v>
       </c>
       <c r="D3" s="3">
-        <v>147.0</v>
+        <v>147</v>
       </c>
       <c r="E3" s="3">
-        <v>70.0</v>
-      </c>
-      <c r="G3" t="str">
+        <v>70</v>
+      </c>
+      <c r="G3">
         <f>Experiment!D3-D3</f>
         <v>-31</v>
       </c>
       <c r="H3" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" t="str">
+      <c r="J3">
         <f>Experiment!E3-E3</f>
         <v>21</v>
       </c>
       <c r="K3" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3">
-        <v>10511.0</v>
+        <v>10511</v>
       </c>
       <c r="C4" s="3">
-        <v>909.0</v>
+        <v>909</v>
       </c>
       <c r="D4" s="3">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="E4" s="3">
-        <v>95.0</v>
-      </c>
-      <c r="G4" t="str">
+        <v>95</v>
+      </c>
+      <c r="G4">
         <f>Experiment!D4-D4</f>
         <v>-22</v>
       </c>
@@ -359,9 +685,9 @@
         <v>12</v>
       </c>
       <c r="I4" s="5">
-        <v>0.0026</v>
-      </c>
-      <c r="J4" t="str">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="J4">
         <f>Experiment!E4-E4</f>
         <v>-16</v>
       </c>
@@ -369,721 +695,768 @@
         <v>12</v>
       </c>
       <c r="L4" s="5">
-        <v>0.6776</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>0.67759999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3">
-        <v>9871.0</v>
+        <v>9871</v>
       </c>
       <c r="C5" s="3">
-        <v>836.0</v>
+        <v>836</v>
       </c>
       <c r="D5" s="3">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="E5" s="3">
-        <v>105.0</v>
-      </c>
-      <c r="G5" t="str">
+        <v>105</v>
+      </c>
+      <c r="G5">
         <f>Experiment!D5-D5</f>
         <v>-18</v>
       </c>
-      <c r="J5" t="str">
+      <c r="J5">
         <f>Experiment!E5-E5</f>
         <v>-13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3">
-        <v>10014.0</v>
+        <v>10014</v>
       </c>
       <c r="C6" s="3">
-        <v>837.0</v>
+        <v>837</v>
       </c>
       <c r="D6" s="3">
-        <v>163.0</v>
+        <v>163</v>
       </c>
       <c r="E6" s="3">
-        <v>64.0</v>
-      </c>
-      <c r="G6" t="str">
+        <v>64</v>
+      </c>
+      <c r="G6">
         <f>Experiment!D6-D6</f>
         <v>-23</v>
       </c>
-      <c r="J6" t="str">
+      <c r="J6">
         <f>Experiment!E6-E6</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>9670.0</v>
+        <v>9670</v>
       </c>
       <c r="C7" s="3">
-        <v>823.0</v>
+        <v>823</v>
       </c>
       <c r="D7" s="3">
-        <v>138.0</v>
+        <v>138</v>
       </c>
       <c r="E7" s="3">
-        <v>82.0</v>
-      </c>
-      <c r="G7" t="str">
+        <v>82</v>
+      </c>
+      <c r="G7">
         <f>Experiment!D7-D7</f>
         <v>-9</v>
       </c>
-      <c r="J7" t="str">
+      <c r="J7">
         <f>Experiment!E7-E7</f>
         <v>-21</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="3">
-        <v>9008.0</v>
+        <v>9008</v>
       </c>
       <c r="C8" s="3">
-        <v>748.0</v>
+        <v>748</v>
       </c>
       <c r="D8" s="3">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="E8" s="3">
-        <v>76.0</v>
-      </c>
-      <c r="G8" t="str">
+        <v>76</v>
+      </c>
+      <c r="G8">
         <f>Experiment!D8-D8</f>
         <v>-19</v>
       </c>
-      <c r="J8" t="str">
+      <c r="J8">
         <f>Experiment!E8-E8</f>
         <v>-32</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3">
-        <v>7434.0</v>
+        <v>7434</v>
       </c>
       <c r="C9" s="3">
-        <v>632.0</v>
+        <v>632</v>
       </c>
       <c r="D9" s="3">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="E9" s="3">
-        <v>70.0</v>
-      </c>
-      <c r="G9" t="str">
+        <v>70</v>
+      </c>
+      <c r="G9">
         <f>Experiment!D9-D9</f>
         <v>-16</v>
       </c>
-      <c r="J9" t="str">
+      <c r="J9">
         <f>Experiment!E9-E9</f>
         <v>-8</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="3">
-        <v>8459.0</v>
+        <v>8459</v>
       </c>
       <c r="C10" s="3">
-        <v>691.0</v>
+        <v>691</v>
       </c>
       <c r="D10" s="3">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="E10" s="3">
-        <v>60.0</v>
-      </c>
-      <c r="G10" t="str">
+        <v>60</v>
+      </c>
+      <c r="G10">
         <f>Experiment!D10-D10</f>
         <v>-11</v>
       </c>
-      <c r="J10" t="str">
+      <c r="J10">
         <f>Experiment!E10-E10</f>
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3">
-        <v>10667.0</v>
+        <v>10667</v>
       </c>
       <c r="C11" s="3">
-        <v>861.0</v>
+        <v>861</v>
       </c>
       <c r="D11" s="3">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="E11" s="3">
-        <v>97.0</v>
-      </c>
-      <c r="G11" t="str">
+        <v>97</v>
+      </c>
+      <c r="G11">
         <f>Experiment!D11-D11</f>
         <v>-12</v>
       </c>
-      <c r="J11" t="str">
+      <c r="J11">
         <f>Experiment!E11-E11</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3">
-        <v>10660.0</v>
+        <v>10660</v>
       </c>
       <c r="C12" s="3">
-        <v>867.0</v>
+        <v>867</v>
       </c>
       <c r="D12" s="3">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="E12" s="3">
-        <v>105.0</v>
-      </c>
-      <c r="G12" t="str">
+        <v>105</v>
+      </c>
+      <c r="G12">
         <f>Experiment!D12-D12</f>
         <v>-53</v>
       </c>
-      <c r="J12" t="str">
+      <c r="J12">
         <f>Experiment!E12-E12</f>
         <v>-34</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="3">
-        <v>9947.0</v>
+        <v>9947</v>
       </c>
       <c r="C13" s="3">
-        <v>838.0</v>
+        <v>838</v>
       </c>
       <c r="D13" s="3">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="E13" s="3">
-        <v>92.0</v>
-      </c>
-      <c r="G13" t="str">
+        <v>92</v>
+      </c>
+      <c r="G13">
         <f>Experiment!D13-D13</f>
         <v>-34</v>
       </c>
-      <c r="J13" t="str">
+      <c r="J13">
         <f>Experiment!E13-E13</f>
         <v>-22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="3">
-        <v>8324.0</v>
+        <v>8324</v>
       </c>
       <c r="C14" s="3">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D14" s="3">
-        <v>127.0</v>
+        <v>127</v>
       </c>
       <c r="E14" s="3">
-        <v>56.0</v>
-      </c>
-      <c r="G14" t="str">
+        <v>56</v>
+      </c>
+      <c r="G14">
         <f>Experiment!D14-D14</f>
         <v>-5</v>
       </c>
-      <c r="J14" t="str">
+      <c r="J14">
         <f>Experiment!E14-E14</f>
         <v>12</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="3">
-        <v>9434.0</v>
+        <v>9434</v>
       </c>
       <c r="C15" s="3">
-        <v>673.0</v>
+        <v>673</v>
       </c>
       <c r="D15" s="3">
-        <v>220.0</v>
+        <v>220</v>
       </c>
       <c r="E15" s="3">
-        <v>122.0</v>
-      </c>
-      <c r="G15" t="str">
+        <v>122</v>
+      </c>
+      <c r="G15">
         <f>Experiment!D15-D15</f>
         <v>-26</v>
       </c>
-      <c r="J15" t="str">
+      <c r="J15">
         <f>Experiment!E15-E15</f>
         <v>-28</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="3">
-        <v>8687.0</v>
+        <v>8687</v>
       </c>
       <c r="C16" s="3">
-        <v>691.0</v>
+        <v>691</v>
       </c>
       <c r="D16" s="3">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="E16" s="3">
-        <v>128.0</v>
-      </c>
-      <c r="G16" t="str">
+        <v>128</v>
+      </c>
+      <c r="G16">
         <f>Experiment!D16-D16</f>
         <v>-49</v>
       </c>
-      <c r="J16" t="str">
+      <c r="J16">
         <f>Experiment!E16-E16</f>
         <v>-47</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="3">
-        <v>8896.0</v>
+        <v>8896</v>
       </c>
       <c r="C17" s="3">
-        <v>708.0</v>
+        <v>708</v>
       </c>
       <c r="D17" s="3">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="E17" s="3">
-        <v>104.0</v>
-      </c>
-      <c r="G17" t="str">
+        <v>104</v>
+      </c>
+      <c r="G17">
         <f>Experiment!D17-D17</f>
         <v>-8</v>
       </c>
-      <c r="J17" t="str">
+      <c r="J17">
         <f>Experiment!E17-E17</f>
         <v>-3</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="3">
-        <v>9535.0</v>
+        <v>9535</v>
       </c>
       <c r="C18" s="3">
-        <v>759.0</v>
+        <v>759</v>
       </c>
       <c r="D18" s="3">
-        <v>233.0</v>
+        <v>233</v>
       </c>
       <c r="E18" s="3">
-        <v>124.0</v>
-      </c>
-      <c r="G18" t="str">
+        <v>124</v>
+      </c>
+      <c r="G18">
         <f>Experiment!D18-D18</f>
         <v>-20</v>
       </c>
-      <c r="J18" t="str">
+      <c r="J18">
         <f>Experiment!E18-E18</f>
         <v>-5</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="3">
-        <v>9363.0</v>
+        <v>9363</v>
       </c>
       <c r="C19" s="3">
-        <v>736.0</v>
+        <v>736</v>
       </c>
       <c r="D19" s="3">
-        <v>154.0</v>
+        <v>154</v>
       </c>
       <c r="E19" s="3">
-        <v>91.0</v>
-      </c>
-      <c r="G19" t="str">
+        <v>91</v>
+      </c>
+      <c r="G19">
         <f>Experiment!D19-D19</f>
         <v>8</v>
       </c>
-      <c r="J19" t="str">
+      <c r="J19">
         <f>Experiment!E19-E19</f>
         <v>29</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="3">
-        <v>9327.0</v>
+        <v>9327</v>
       </c>
       <c r="C20" s="3">
-        <v>739.0</v>
+        <v>739</v>
       </c>
       <c r="D20" s="3">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="E20" s="3">
-        <v>86.0</v>
-      </c>
-      <c r="G20" t="str">
+        <v>86</v>
+      </c>
+      <c r="G20">
         <f>Experiment!D20-D20</f>
         <v>5</v>
       </c>
-      <c r="J20" t="str">
+      <c r="J20">
         <f>Experiment!E20-E20</f>
         <v>10</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="3">
-        <v>9345.0</v>
+        <v>9345</v>
       </c>
       <c r="C21" s="3">
-        <v>734.0</v>
+        <v>734</v>
       </c>
       <c r="D21" s="3">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="E21" s="3">
-        <v>75.0</v>
-      </c>
-      <c r="G21" t="str">
+        <v>75</v>
+      </c>
+      <c r="G21">
         <f>Experiment!D21-D21</f>
         <v>40</v>
       </c>
-      <c r="J21" t="str">
+      <c r="J21">
         <f>Experiment!E21-E21</f>
         <v>-8</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3">
-        <v>8890.0</v>
+        <v>8890</v>
       </c>
       <c r="C22" s="3">
-        <v>706.0</v>
+        <v>706</v>
       </c>
       <c r="D22" s="3">
-        <v>174.0</v>
+        <v>174</v>
       </c>
       <c r="E22" s="3">
-        <v>101.0</v>
-      </c>
-      <c r="G22" t="str">
+        <v>101</v>
+      </c>
+      <c r="G22">
         <f>Experiment!D22-D22</f>
         <v>8</v>
       </c>
-      <c r="J22" t="str">
+      <c r="J22">
         <f>Experiment!E22-E22</f>
         <v>22</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="3">
-        <v>8460.0</v>
+        <v>8460</v>
       </c>
       <c r="C23" s="3">
-        <v>681.0</v>
+        <v>681</v>
       </c>
       <c r="D23" s="3">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="E23" s="3">
-        <v>93.0</v>
-      </c>
-      <c r="G23" t="str">
+        <v>93</v>
+      </c>
+      <c r="G23">
         <f>Experiment!D23-D23</f>
         <v>-14</v>
       </c>
-      <c r="J23" t="str">
+      <c r="J23">
         <f>Experiment!E23-E23</f>
         <v>7</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="3">
-        <v>8836.0</v>
+        <v>8836</v>
       </c>
       <c r="C24" s="3">
-        <v>693.0</v>
+        <v>693</v>
       </c>
       <c r="D24" s="3">
-        <v>206.0</v>
+        <v>206</v>
       </c>
       <c r="E24" s="3">
-        <v>67.0</v>
-      </c>
-      <c r="G24" t="str">
+        <v>67</v>
+      </c>
+      <c r="G24">
         <f>Experiment!D24-D24</f>
         <v>-24</v>
       </c>
-      <c r="J24" t="str">
+      <c r="J24">
         <f>Experiment!E24-E24</f>
         <v>36</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="3">
-        <v>9437.0</v>
+        <v>9437</v>
       </c>
       <c r="C25" s="3">
-        <v>788.0</v>
+        <v>788</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="3">
-        <v>9420.0</v>
+        <v>9420</v>
       </c>
       <c r="C26" s="3">
-        <v>781.0</v>
+        <v>781</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="3">
-        <v>9570.0</v>
+        <v>9570</v>
       </c>
       <c r="C27" s="3">
-        <v>805.0</v>
+        <v>805</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="3">
-        <v>9921.0</v>
+        <v>9921</v>
       </c>
       <c r="C28" s="3">
-        <v>830.0</v>
+        <v>830</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="3">
-        <v>9424.0</v>
+        <v>9424</v>
       </c>
       <c r="C29" s="3">
-        <v>781.0</v>
+        <v>781</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="3">
-        <v>9010.0</v>
+        <v>9010</v>
       </c>
       <c r="C30" s="3">
-        <v>756.0</v>
+        <v>756</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="3">
-        <v>9656.0</v>
+        <v>9656</v>
       </c>
       <c r="C31" s="3">
-        <v>825.0</v>
+        <v>825</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="3">
-        <v>10419.0</v>
+        <v>10419</v>
       </c>
       <c r="C32" s="3">
-        <v>874.0</v>
+        <v>874</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="3">
-        <v>9880.0</v>
+        <v>9880</v>
       </c>
       <c r="C33" s="3">
-        <v>830.0</v>
+        <v>830</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34">
+      <c r="E33" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="3">
-        <v>10134.0</v>
+        <v>10134</v>
       </c>
       <c r="C34" s="3">
-        <v>801.0</v>
+        <v>801</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35">
+      <c r="E34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34">
+        <f>C40/B40</f>
+        <v>8.2125813574576823E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B35" s="3">
-        <v>9717.0</v>
+        <v>9717</v>
       </c>
       <c r="C35" s="3">
-        <v>814.0</v>
+        <v>814</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36">
+      <c r="E35" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35">
+        <f>SQRT(F34*(1-F34)/B40)</f>
+        <v>4.6706827655464432E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="3">
-        <v>9192.0</v>
+        <v>9192</v>
       </c>
       <c r="C36" s="3">
-        <v>735.0</v>
+        <v>735</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37">
+      <c r="E36" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36">
+        <f>F35*1.96</f>
+        <v>9.154538220471028E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="3">
-        <v>8630.0</v>
+        <v>8630</v>
       </c>
       <c r="C37" s="3">
-        <v>743.0</v>
+        <v>743</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38">
+      <c r="E37" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <f>F34-F36</f>
+        <v>8.1210359752529715E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="3">
-        <v>8970.0</v>
+        <v>8970</v>
       </c>
       <c r="C38" s="3">
-        <v>722.0</v>
+        <v>722</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39">
+      <c r="E38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38">
+        <f>F36+F34</f>
+        <v>8.304126739662393E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40">
-      <c r="A40" s="1"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="3">
+        <f>SUM(B2:B38)</f>
+        <v>345543</v>
+      </c>
+      <c r="C40" s="3">
+        <f>SUM(C2:C38)</f>
+        <v>28378</v>
+      </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="6"/>
+      <c r="E40" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40">
+        <f>Experiment!C40/Experiment!B40</f>
+        <v>8.2182440666163759E-2</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1100,580 +1473,593 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>7716.0</v>
+        <v>7716</v>
       </c>
       <c r="C2" s="3">
-        <v>686.0</v>
+        <v>686</v>
       </c>
       <c r="D2" s="3">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="E2" s="3">
-        <v>34.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3">
-        <v>9288.0</v>
+        <v>9288</v>
       </c>
       <c r="C3" s="3">
-        <v>785.0</v>
+        <v>785</v>
       </c>
       <c r="D3" s="3">
-        <v>116.0</v>
+        <v>116</v>
       </c>
       <c r="E3" s="3">
-        <v>91.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3">
-        <v>10480.0</v>
+        <v>10480</v>
       </c>
       <c r="C4" s="3">
-        <v>884.0</v>
+        <v>884</v>
       </c>
       <c r="D4" s="3">
-        <v>145.0</v>
+        <v>145</v>
       </c>
       <c r="E4" s="3">
-        <v>79.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3">
-        <v>9867.0</v>
+        <v>9867</v>
       </c>
       <c r="C5" s="3">
-        <v>827.0</v>
+        <v>827</v>
       </c>
       <c r="D5" s="3">
-        <v>138.0</v>
+        <v>138</v>
       </c>
       <c r="E5" s="3">
-        <v>92.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3">
-        <v>9793.0</v>
+        <v>9793</v>
       </c>
       <c r="C6" s="3">
-        <v>832.0</v>
+        <v>832</v>
       </c>
       <c r="D6" s="3">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="E6" s="3">
-        <v>94.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>9500.0</v>
+        <v>9500</v>
       </c>
       <c r="C7" s="3">
-        <v>788.0</v>
+        <v>788</v>
       </c>
       <c r="D7" s="3">
-        <v>129.0</v>
+        <v>129</v>
       </c>
       <c r="E7" s="3">
-        <v>61.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="3">
-        <v>9088.0</v>
+        <v>9088</v>
       </c>
       <c r="C8" s="3">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D8" s="3">
-        <v>127.0</v>
+        <v>127</v>
       </c>
       <c r="E8" s="3">
-        <v>44.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3">
-        <v>7664.0</v>
+        <v>7664</v>
       </c>
       <c r="C9" s="3">
-        <v>652.0</v>
+        <v>652</v>
       </c>
       <c r="D9" s="3">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="E9" s="3">
-        <v>62.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="3">
-        <v>8434.0</v>
+        <v>8434</v>
       </c>
       <c r="C10" s="3">
-        <v>697.0</v>
+        <v>697</v>
       </c>
       <c r="D10" s="3">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="E10" s="3">
-        <v>77.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3">
-        <v>10496.0</v>
+        <v>10496</v>
       </c>
       <c r="C11" s="3">
-        <v>860.0</v>
+        <v>860</v>
       </c>
       <c r="D11" s="3">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="E11" s="3">
-        <v>98.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3">
-        <v>10551.0</v>
+        <v>10551</v>
       </c>
       <c r="C12" s="3">
-        <v>864.0</v>
+        <v>864</v>
       </c>
       <c r="D12" s="3">
-        <v>143.0</v>
+        <v>143</v>
       </c>
       <c r="E12" s="3">
-        <v>71.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="3">
-        <v>9737.0</v>
+        <v>9737</v>
       </c>
       <c r="C13" s="3">
-        <v>801.0</v>
+        <v>801</v>
       </c>
       <c r="D13" s="3">
-        <v>128.0</v>
+        <v>128</v>
       </c>
       <c r="E13" s="3">
-        <v>70.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="3">
-        <v>8176.0</v>
+        <v>8176</v>
       </c>
       <c r="C14" s="3">
-        <v>642.0</v>
+        <v>642</v>
       </c>
       <c r="D14" s="3">
-        <v>122.0</v>
+        <v>122</v>
       </c>
       <c r="E14" s="3">
-        <v>68.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="3">
-        <v>9402.0</v>
+        <v>9402</v>
       </c>
       <c r="C15" s="3">
-        <v>697.0</v>
+        <v>697</v>
       </c>
       <c r="D15" s="3">
-        <v>194.0</v>
+        <v>194</v>
       </c>
       <c r="E15" s="3">
-        <v>94.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="3">
-        <v>8669.0</v>
+        <v>8669</v>
       </c>
       <c r="C16" s="3">
-        <v>669.0</v>
+        <v>669</v>
       </c>
       <c r="D16" s="3">
-        <v>127.0</v>
+        <v>127</v>
       </c>
       <c r="E16" s="3">
-        <v>81.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="3">
-        <v>8881.0</v>
+        <v>8881</v>
       </c>
       <c r="C17" s="3">
-        <v>693.0</v>
+        <v>693</v>
       </c>
       <c r="D17" s="3">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="E17" s="3">
-        <v>101.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="3">
-        <v>9655.0</v>
+        <v>9655</v>
       </c>
       <c r="C18" s="3">
-        <v>771.0</v>
+        <v>771</v>
       </c>
       <c r="D18" s="3">
-        <v>213.0</v>
+        <v>213</v>
       </c>
       <c r="E18" s="3">
-        <v>119.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="3">
-        <v>9396.0</v>
+        <v>9396</v>
       </c>
       <c r="C19" s="3">
-        <v>736.0</v>
+        <v>736</v>
       </c>
       <c r="D19" s="3">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="E19" s="3">
-        <v>120.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="3">
-        <v>9262.0</v>
+        <v>9262</v>
       </c>
       <c r="C20" s="3">
-        <v>727.0</v>
+        <v>727</v>
       </c>
       <c r="D20" s="3">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="E20" s="3">
-        <v>96.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="3">
-        <v>9308.0</v>
+        <v>9308</v>
       </c>
       <c r="C21" s="3">
-        <v>728.0</v>
+        <v>728</v>
       </c>
       <c r="D21" s="3">
-        <v>207.0</v>
+        <v>207</v>
       </c>
       <c r="E21" s="3">
-        <v>67.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3">
-        <v>8715.0</v>
+        <v>8715</v>
       </c>
       <c r="C22" s="3">
-        <v>722.0</v>
+        <v>722</v>
       </c>
       <c r="D22" s="3">
-        <v>182.0</v>
+        <v>182</v>
       </c>
       <c r="E22" s="3">
-        <v>123.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="3">
-        <v>8448.0</v>
+        <v>8448</v>
       </c>
       <c r="C23" s="3">
-        <v>695.0</v>
+        <v>695</v>
       </c>
       <c r="D23" s="3">
-        <v>142.0</v>
+        <v>142</v>
       </c>
       <c r="E23" s="3">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="3">
-        <v>8836.0</v>
+        <v>8836</v>
       </c>
       <c r="C24" s="3">
-        <v>724.0</v>
+        <v>724</v>
       </c>
       <c r="D24" s="3">
-        <v>182.0</v>
+        <v>182</v>
       </c>
       <c r="E24" s="3">
-        <v>103.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="3">
-        <v>9359.0</v>
+        <v>9359</v>
       </c>
       <c r="C25" s="3">
-        <v>789.0</v>
+        <v>789</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="3">
-        <v>9427.0</v>
+        <v>9427</v>
       </c>
       <c r="C26" s="3">
-        <v>743.0</v>
+        <v>743</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="3">
-        <v>9633.0</v>
+        <v>9633</v>
       </c>
       <c r="C27" s="3">
-        <v>808.0</v>
+        <v>808</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="3">
-        <v>9842.0</v>
+        <v>9842</v>
       </c>
       <c r="C28" s="3">
-        <v>831.0</v>
+        <v>831</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="3">
-        <v>9272.0</v>
+        <v>9272</v>
       </c>
       <c r="C29" s="3">
-        <v>767.0</v>
+        <v>767</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="3">
-        <v>8969.0</v>
+        <v>8969</v>
       </c>
       <c r="C30" s="3">
-        <v>760.0</v>
+        <v>760</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="3">
-        <v>9697.0</v>
+        <v>9697</v>
       </c>
       <c r="C31" s="3">
-        <v>850.0</v>
+        <v>850</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="3">
-        <v>10445.0</v>
+        <v>10445</v>
       </c>
       <c r="C32" s="3">
-        <v>851.0</v>
+        <v>851</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="3">
-        <v>9931.0</v>
+        <v>9931</v>
       </c>
       <c r="C33" s="3">
-        <v>831.0</v>
+        <v>831</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="3">
-        <v>10042.0</v>
+        <v>10042</v>
       </c>
       <c r="C34" s="3">
-        <v>802.0</v>
+        <v>802</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B35" s="3">
-        <v>9721.0</v>
+        <v>9721</v>
       </c>
       <c r="C35" s="3">
-        <v>829.0</v>
+        <v>829</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="3">
-        <v>9304.0</v>
+        <v>9304</v>
       </c>
       <c r="C36" s="3">
-        <v>770.0</v>
+        <v>770</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="3">
-        <v>8668.0</v>
+        <v>8668</v>
       </c>
       <c r="C37" s="3">
-        <v>724.0</v>
+        <v>724</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="3">
-        <v>8988.0</v>
+        <v>8988</v>
       </c>
       <c r="C38" s="3">
-        <v>710.0</v>
+        <v>710</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="3">
+        <f>SUM(B2:B38)</f>
+        <v>344660</v>
+      </c>
+      <c r="C40" s="3">
+        <f>SUM(C2:C38)</f>
+        <v>28325</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>